<commit_message>
Generalizing coffee to plant in company-farmer-details page, updated list of farmers template
</commit_message>
<xml_diff>
--- a/src/assets/farmer-import/Template_list of farmers_NEW.xlsx
+++ b/src/assets/farmer-import/Template_list of farmers_NEW.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11012"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nejc\Documents\Work\Sunesis\INAtrace\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bpaspalovski/IntellijProjects/inatrace/inatrace-fe/src/assets/farmer-import/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F23D985B-1E26-43A6-BC8A-A7F8BB534B5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3CA0E02-6116-994D-B698-073674D4EC32}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3440" yWindow="500" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -48,9 +48,6 @@
   </si>
   <si>
     <t>E-mail</t>
-  </si>
-  <si>
-    <t>Number of coffee trees</t>
   </si>
   <si>
     <t>Bank name</t>
@@ -119,9 +116,6 @@
     <t>Total cultivated area</t>
   </si>
   <si>
-    <t>Area cultivated with coffee</t>
-  </si>
-  <si>
     <t>Area organic certified</t>
   </si>
   <si>
@@ -149,6 +143,12 @@
       </rPr>
       <t xml:space="preserve"> to organic</t>
     </r>
+  </si>
+  <si>
+    <t>Area cultivated with plant</t>
+  </si>
+  <si>
+    <t>Number of plants</t>
   </si>
 </sst>
 </file>
@@ -358,9 +358,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="24" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -380,33 +377,36 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="25">
-    <cellStyle name="Hiperpovezava" xfId="6" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperpovezava" xfId="8" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperpovezava" xfId="10" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperpovezava" xfId="12" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperpovezava" xfId="14" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperpovezava" xfId="16" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperpovezava" xfId="18" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperpovezava" xfId="20" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperpovezava" xfId="22" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperpovezava" xfId="24" builtinId="8"/>
-    <cellStyle name="Navadno" xfId="0" builtinId="0"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="23" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="12" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="14" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="16" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="18" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="20" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="22" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="24" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
     <cellStyle name="Normal 2 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
     <cellStyle name="Normal 2 3" xfId="3" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
     <cellStyle name="Normal 2 4" xfId="4" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
     <cellStyle name="Normal 2 5" xfId="5" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
-    <cellStyle name="Obiskana hiperpovezava" xfId="7" builtinId="9" hidden="1"/>
-    <cellStyle name="Obiskana hiperpovezava" xfId="9" builtinId="9" hidden="1"/>
-    <cellStyle name="Obiskana hiperpovezava" xfId="11" builtinId="9" hidden="1"/>
-    <cellStyle name="Obiskana hiperpovezava" xfId="13" builtinId="9" hidden="1"/>
-    <cellStyle name="Obiskana hiperpovezava" xfId="15" builtinId="9" hidden="1"/>
-    <cellStyle name="Obiskana hiperpovezava" xfId="17" builtinId="9" hidden="1"/>
-    <cellStyle name="Obiskana hiperpovezava" xfId="19" builtinId="9" hidden="1"/>
-    <cellStyle name="Obiskana hiperpovezava" xfId="21" builtinId="9" hidden="1"/>
-    <cellStyle name="Obiskana hiperpovezava" xfId="23" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -422,9 +422,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Officeova tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Pisarna">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -462,7 +462,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Pisarna">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -568,7 +568,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Pisarna">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -744,54 +744,54 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AL260"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="AJ5" sqref="AJ5"/>
+    <sheetView tabSelected="1" topLeftCell="U1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="Y10" sqref="Y10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="25.33203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="17" style="1" customWidth="1"/>
-    <col min="3" max="3" width="26.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="23.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="22.28515625" style="1" customWidth="1"/>
-    <col min="6" max="14" width="19.85546875" style="1" customWidth="1"/>
-    <col min="15" max="15" width="29.140625" customWidth="1"/>
-    <col min="16" max="16" width="29.140625" style="1" customWidth="1"/>
-    <col min="17" max="17" width="17.140625" customWidth="1"/>
-    <col min="18" max="18" width="19.7109375" style="1" customWidth="1"/>
-    <col min="19" max="19" width="18.28515625" style="1" customWidth="1"/>
-    <col min="20" max="20" width="15.85546875" style="1" customWidth="1"/>
-    <col min="21" max="22" width="26.42578125" style="1" customWidth="1"/>
-    <col min="23" max="27" width="18.28515625" style="1" customWidth="1"/>
-    <col min="28" max="28" width="20.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="26.1640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="23.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="22.33203125" style="1" customWidth="1"/>
+    <col min="6" max="14" width="19.83203125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="29.1640625" customWidth="1"/>
+    <col min="16" max="16" width="29.1640625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="17.1640625" customWidth="1"/>
+    <col min="18" max="18" width="19.6640625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="18.33203125" style="1" customWidth="1"/>
+    <col min="20" max="20" width="15.83203125" style="1" customWidth="1"/>
+    <col min="21" max="22" width="26.5" style="1" customWidth="1"/>
+    <col min="23" max="27" width="18.33203125" style="1" customWidth="1"/>
+    <col min="28" max="28" width="20.5" style="1" customWidth="1"/>
     <col min="29" max="29" width="26" customWidth="1"/>
-    <col min="30" max="30" width="21.140625" customWidth="1"/>
-    <col min="31" max="31" width="25.42578125" customWidth="1"/>
-    <col min="32" max="32" width="22.7109375" customWidth="1"/>
+    <col min="30" max="30" width="21.1640625" customWidth="1"/>
+    <col min="31" max="31" width="25.5" customWidth="1"/>
+    <col min="32" max="32" width="22.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:38" x14ac:dyDescent="0.2">
       <c r="O1" s="1"/>
       <c r="Q1" s="1"/>
     </row>
-    <row r="2" spans="1:38" ht="26.25" x14ac:dyDescent="0.3">
-      <c r="C2" s="20" t="s">
+    <row r="2" spans="1:38" ht="26" x14ac:dyDescent="0.25">
+      <c r="C2" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
-      <c r="J2" s="21"/>
-      <c r="K2" s="21"/>
-      <c r="L2" s="21"/>
-      <c r="M2" s="21"/>
-      <c r="N2" s="21"/>
-      <c r="O2" s="21"/>
-      <c r="P2" s="22"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
+      <c r="L2" s="20"/>
+      <c r="M2" s="20"/>
+      <c r="N2" s="20"/>
+      <c r="O2" s="20"/>
+      <c r="P2" s="21"/>
       <c r="R2" s="3"/>
       <c r="S2" s="3"/>
       <c r="T2" s="3"/>
@@ -804,120 +804,120 @@
       <c r="AA2" s="3"/>
       <c r="AB2" s="3"/>
     </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:38" x14ac:dyDescent="0.2">
       <c r="O3" s="1"/>
       <c r="Q3" s="1"/>
     </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:38" x14ac:dyDescent="0.2">
       <c r="D4" s="16"/>
       <c r="O4" s="1"/>
       <c r="Q4" s="1"/>
     </row>
-    <row r="5" spans="1:38" s="27" customFormat="1" ht="63.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="23" t="s">
+    <row r="5" spans="1:38" s="26" customFormat="1" ht="64" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="23" t="s">
+      <c r="D5" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="23" t="s">
+      <c r="F5" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="23" t="s">
+      <c r="G5" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="J5" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="K5" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="L5" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="M5" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="N5" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="O5" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="P5" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q5" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="R5" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="S5" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="T5" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="U5" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="V5" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="W5" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="X5" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y5" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z5" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="H5" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="I5" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="J5" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="K5" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="L5" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="M5" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="N5" s="23" t="s">
-        <v>19</v>
-      </c>
-      <c r="O5" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="P5" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q5" s="24" t="s">
-        <v>5</v>
-      </c>
-      <c r="R5" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="S5" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="T5" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="U5" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="V5" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="W5" s="23" t="s">
+      <c r="AA5" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="X5" s="23" t="s">
+      <c r="AB5" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="Y5" s="23" t="s">
+      <c r="AC5" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="AD5" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="AE5" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="Z5" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="AA5" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="AB5" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="AC5" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="AD5" s="25" t="s">
+      <c r="AF5" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="AE5" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="AF5" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="AG5" s="26"/>
-      <c r="AH5" s="26"/>
-      <c r="AI5" s="26"/>
-      <c r="AJ5" s="26"/>
-      <c r="AK5" s="26"/>
-      <c r="AL5" s="26"/>
-    </row>
-    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AG5" s="25"/>
+      <c r="AH5" s="25"/>
+      <c r="AI5" s="25"/>
+      <c r="AJ5" s="25"/>
+      <c r="AK5" s="25"/>
+      <c r="AL5" s="25"/>
+    </row>
+    <row r="6" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -957,7 +957,7 @@
       <c r="AK6" s="10"/>
       <c r="AL6" s="10"/>
     </row>
-    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -997,7 +997,7 @@
       <c r="AK7" s="10"/>
       <c r="AL7" s="10"/>
     </row>
-    <row r="8" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -1037,7 +1037,7 @@
       <c r="AK8" s="10"/>
       <c r="AL8" s="10"/>
     </row>
-    <row r="9" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="B9" s="4"/>
       <c r="C9" s="2"/>
@@ -1077,7 +1077,7 @@
       <c r="AK9" s="10"/>
       <c r="AL9" s="10"/>
     </row>
-    <row r="10" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -1117,7 +1117,7 @@
       <c r="AK10" s="10"/>
       <c r="AL10" s="10"/>
     </row>
-    <row r="11" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -1157,7 +1157,7 @@
       <c r="AK11" s="10"/>
       <c r="AL11" s="10"/>
     </row>
-    <row r="12" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -1197,7 +1197,7 @@
       <c r="AK12" s="10"/>
       <c r="AL12" s="10"/>
     </row>
-    <row r="13" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
       <c r="B13" s="4"/>
       <c r="C13" s="2"/>
@@ -1237,7 +1237,7 @@
       <c r="AK13" s="10"/>
       <c r="AL13" s="10"/>
     </row>
-    <row r="14" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -1277,7 +1277,7 @@
       <c r="AK14" s="10"/>
       <c r="AL14" s="10"/>
     </row>
-    <row r="15" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -1317,7 +1317,7 @@
       <c r="AK15" s="10"/>
       <c r="AL15" s="10"/>
     </row>
-    <row r="16" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -1357,7 +1357,7 @@
       <c r="AK16" s="10"/>
       <c r="AL16" s="10"/>
     </row>
-    <row r="17" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
       <c r="B17" s="4"/>
       <c r="C17" s="2"/>
@@ -1397,7 +1397,7 @@
       <c r="AK17" s="10"/>
       <c r="AL17" s="10"/>
     </row>
-    <row r="18" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -1437,7 +1437,7 @@
       <c r="AK18" s="10"/>
       <c r="AL18" s="10"/>
     </row>
-    <row r="19" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -1477,7 +1477,7 @@
       <c r="AK19" s="10"/>
       <c r="AL19" s="10"/>
     </row>
-    <row r="20" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -1517,7 +1517,7 @@
       <c r="AK20" s="10"/>
       <c r="AL20" s="10"/>
     </row>
-    <row r="21" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A21" s="2"/>
       <c r="B21" s="4"/>
       <c r="C21" s="2"/>
@@ -1557,7 +1557,7 @@
       <c r="AK21" s="10"/>
       <c r="AL21" s="10"/>
     </row>
-    <row r="22" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -1597,7 +1597,7 @@
       <c r="AK22" s="10"/>
       <c r="AL22" s="10"/>
     </row>
-    <row r="23" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -1637,7 +1637,7 @@
       <c r="AK23" s="10"/>
       <c r="AL23" s="10"/>
     </row>
-    <row r="24" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -1677,7 +1677,7 @@
       <c r="AK24" s="10"/>
       <c r="AL24" s="10"/>
     </row>
-    <row r="25" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A25" s="2"/>
       <c r="B25" s="4"/>
       <c r="C25" s="2"/>
@@ -1717,7 +1717,7 @@
       <c r="AK25" s="10"/>
       <c r="AL25" s="10"/>
     </row>
-    <row r="26" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -1757,7 +1757,7 @@
       <c r="AK26" s="10"/>
       <c r="AL26" s="10"/>
     </row>
-    <row r="27" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -1797,7 +1797,7 @@
       <c r="AK27" s="10"/>
       <c r="AL27" s="10"/>
     </row>
-    <row r="28" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -1837,7 +1837,7 @@
       <c r="AK28" s="10"/>
       <c r="AL28" s="10"/>
     </row>
-    <row r="29" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A29" s="2"/>
       <c r="B29" s="4"/>
       <c r="C29" s="2"/>
@@ -1877,7 +1877,7 @@
       <c r="AK29" s="10"/>
       <c r="AL29" s="10"/>
     </row>
-    <row r="30" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -1917,7 +1917,7 @@
       <c r="AK30" s="10"/>
       <c r="AL30" s="10"/>
     </row>
-    <row r="31" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -1957,7 +1957,7 @@
       <c r="AK31" s="10"/>
       <c r="AL31" s="10"/>
     </row>
-    <row r="32" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -1997,7 +1997,7 @@
       <c r="AK32" s="10"/>
       <c r="AL32" s="10"/>
     </row>
-    <row r="33" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A33" s="2"/>
       <c r="B33" s="4"/>
       <c r="C33" s="2"/>
@@ -2037,7 +2037,7 @@
       <c r="AK33" s="10"/>
       <c r="AL33" s="10"/>
     </row>
-    <row r="34" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
@@ -2077,7 +2077,7 @@
       <c r="AK34" s="10"/>
       <c r="AL34" s="10"/>
     </row>
-    <row r="35" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -2117,7 +2117,7 @@
       <c r="AK35" s="10"/>
       <c r="AL35" s="10"/>
     </row>
-    <row r="36" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -2157,7 +2157,7 @@
       <c r="AK36" s="10"/>
       <c r="AL36" s="10"/>
     </row>
-    <row r="37" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A37" s="2"/>
       <c r="B37" s="4"/>
       <c r="C37" s="2"/>
@@ -2197,7 +2197,7 @@
       <c r="AK37" s="10"/>
       <c r="AL37" s="10"/>
     </row>
-    <row r="38" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -2237,7 +2237,7 @@
       <c r="AK38" s="10"/>
       <c r="AL38" s="10"/>
     </row>
-    <row r="39" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
@@ -2277,7 +2277,7 @@
       <c r="AK39" s="10"/>
       <c r="AL39" s="10"/>
     </row>
-    <row r="40" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
@@ -2317,7 +2317,7 @@
       <c r="AK40" s="10"/>
       <c r="AL40" s="10"/>
     </row>
-    <row r="41" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A41" s="2"/>
       <c r="B41" s="4"/>
       <c r="C41" s="2"/>
@@ -2357,7 +2357,7 @@
       <c r="AK41" s="10"/>
       <c r="AL41" s="10"/>
     </row>
-    <row r="42" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
@@ -2397,7 +2397,7 @@
       <c r="AK42" s="10"/>
       <c r="AL42" s="10"/>
     </row>
-    <row r="43" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -2437,7 +2437,7 @@
       <c r="AK43" s="10"/>
       <c r="AL43" s="10"/>
     </row>
-    <row r="44" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
@@ -2477,7 +2477,7 @@
       <c r="AK44" s="10"/>
       <c r="AL44" s="10"/>
     </row>
-    <row r="45" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A45" s="2"/>
       <c r="B45" s="4"/>
       <c r="C45" s="2"/>
@@ -2517,7 +2517,7 @@
       <c r="AK45" s="10"/>
       <c r="AL45" s="10"/>
     </row>
-    <row r="46" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -2557,7 +2557,7 @@
       <c r="AK46" s="10"/>
       <c r="AL46" s="10"/>
     </row>
-    <row r="47" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
@@ -2597,7 +2597,7 @@
       <c r="AK47" s="10"/>
       <c r="AL47" s="10"/>
     </row>
-    <row r="48" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
@@ -2637,7 +2637,7 @@
       <c r="AK48" s="10"/>
       <c r="AL48" s="10"/>
     </row>
-    <row r="49" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A49" s="2"/>
       <c r="B49" s="4"/>
       <c r="C49" s="2"/>
@@ -2677,7 +2677,7 @@
       <c r="AK49" s="10"/>
       <c r="AL49" s="10"/>
     </row>
-    <row r="50" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
@@ -2717,7 +2717,7 @@
       <c r="AK50" s="10"/>
       <c r="AL50" s="10"/>
     </row>
-    <row r="51" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
@@ -2757,7 +2757,7 @@
       <c r="AK51" s="10"/>
       <c r="AL51" s="10"/>
     </row>
-    <row r="52" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
@@ -2797,7 +2797,7 @@
       <c r="AK52" s="10"/>
       <c r="AL52" s="10"/>
     </row>
-    <row r="53" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A53" s="2"/>
       <c r="B53" s="4"/>
       <c r="C53" s="2"/>
@@ -2837,7 +2837,7 @@
       <c r="AK53" s="10"/>
       <c r="AL53" s="10"/>
     </row>
-    <row r="54" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A54" s="2"/>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
@@ -2877,7 +2877,7 @@
       <c r="AK54" s="10"/>
       <c r="AL54" s="10"/>
     </row>
-    <row r="55" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A55" s="2"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
@@ -2917,7 +2917,7 @@
       <c r="AK55" s="10"/>
       <c r="AL55" s="10"/>
     </row>
-    <row r="56" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A56" s="2"/>
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
@@ -2957,7 +2957,7 @@
       <c r="AK56" s="10"/>
       <c r="AL56" s="10"/>
     </row>
-    <row r="57" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A57" s="2"/>
       <c r="B57" s="4"/>
       <c r="C57" s="2"/>
@@ -2997,7 +2997,7 @@
       <c r="AK57" s="10"/>
       <c r="AL57" s="10"/>
     </row>
-    <row r="58" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A58" s="2"/>
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
@@ -3037,7 +3037,7 @@
       <c r="AK58" s="10"/>
       <c r="AL58" s="10"/>
     </row>
-    <row r="59" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A59" s="2"/>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
@@ -3077,7 +3077,7 @@
       <c r="AK59" s="10"/>
       <c r="AL59" s="10"/>
     </row>
-    <row r="60" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A60" s="2"/>
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
@@ -3117,7 +3117,7 @@
       <c r="AK60" s="10"/>
       <c r="AL60" s="10"/>
     </row>
-    <row r="61" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A61" s="2"/>
       <c r="B61" s="4"/>
       <c r="C61" s="2"/>
@@ -3157,7 +3157,7 @@
       <c r="AK61" s="10"/>
       <c r="AL61" s="10"/>
     </row>
-    <row r="62" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A62" s="2"/>
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
@@ -3197,7 +3197,7 @@
       <c r="AK62" s="10"/>
       <c r="AL62" s="10"/>
     </row>
-    <row r="63" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A63" s="2"/>
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
@@ -3237,7 +3237,7 @@
       <c r="AK63" s="10"/>
       <c r="AL63" s="10"/>
     </row>
-    <row r="64" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A64" s="2"/>
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
@@ -3277,7 +3277,7 @@
       <c r="AK64" s="10"/>
       <c r="AL64" s="10"/>
     </row>
-    <row r="65" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A65" s="2"/>
       <c r="B65" s="4"/>
       <c r="C65" s="2"/>
@@ -3317,7 +3317,7 @@
       <c r="AK65" s="10"/>
       <c r="AL65" s="10"/>
     </row>
-    <row r="66" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A66" s="2"/>
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
@@ -3357,7 +3357,7 @@
       <c r="AK66" s="10"/>
       <c r="AL66" s="10"/>
     </row>
-    <row r="67" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A67" s="2"/>
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
@@ -3397,7 +3397,7 @@
       <c r="AK67" s="10"/>
       <c r="AL67" s="10"/>
     </row>
-    <row r="68" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A68" s="2"/>
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
@@ -3437,7 +3437,7 @@
       <c r="AK68" s="10"/>
       <c r="AL68" s="10"/>
     </row>
-    <row r="69" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A69" s="2"/>
       <c r="B69" s="4"/>
       <c r="C69" s="2"/>
@@ -3477,7 +3477,7 @@
       <c r="AK69" s="10"/>
       <c r="AL69" s="10"/>
     </row>
-    <row r="70" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A70" s="2"/>
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
@@ -3517,7 +3517,7 @@
       <c r="AK70" s="10"/>
       <c r="AL70" s="10"/>
     </row>
-    <row r="71" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A71" s="2"/>
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
@@ -3557,7 +3557,7 @@
       <c r="AK71" s="10"/>
       <c r="AL71" s="10"/>
     </row>
-    <row r="72" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A72" s="2"/>
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
@@ -3597,7 +3597,7 @@
       <c r="AK72" s="10"/>
       <c r="AL72" s="10"/>
     </row>
-    <row r="73" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A73" s="2"/>
       <c r="B73" s="4"/>
       <c r="C73" s="2"/>
@@ -3637,7 +3637,7 @@
       <c r="AK73" s="10"/>
       <c r="AL73" s="10"/>
     </row>
-    <row r="74" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A74" s="2"/>
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
@@ -3677,7 +3677,7 @@
       <c r="AK74" s="10"/>
       <c r="AL74" s="10"/>
     </row>
-    <row r="75" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A75" s="2"/>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
@@ -3717,7 +3717,7 @@
       <c r="AK75" s="10"/>
       <c r="AL75" s="10"/>
     </row>
-    <row r="76" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A76" s="2"/>
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
@@ -3757,7 +3757,7 @@
       <c r="AK76" s="10"/>
       <c r="AL76" s="10"/>
     </row>
-    <row r="77" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A77" s="2"/>
       <c r="B77" s="4"/>
       <c r="C77" s="2"/>
@@ -3797,7 +3797,7 @@
       <c r="AK77" s="10"/>
       <c r="AL77" s="10"/>
     </row>
-    <row r="78" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A78" s="2"/>
       <c r="B78" s="2"/>
       <c r="C78" s="2"/>
@@ -3837,7 +3837,7 @@
       <c r="AK78" s="10"/>
       <c r="AL78" s="10"/>
     </row>
-    <row r="79" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A79" s="2"/>
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
@@ -3877,7 +3877,7 @@
       <c r="AK79" s="10"/>
       <c r="AL79" s="10"/>
     </row>
-    <row r="80" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A80" s="2"/>
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
@@ -3917,7 +3917,7 @@
       <c r="AK80" s="10"/>
       <c r="AL80" s="10"/>
     </row>
-    <row r="81" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A81" s="2"/>
       <c r="B81" s="4"/>
       <c r="C81" s="2"/>
@@ -3957,7 +3957,7 @@
       <c r="AK81" s="10"/>
       <c r="AL81" s="10"/>
     </row>
-    <row r="82" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A82" s="2"/>
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
@@ -3997,7 +3997,7 @@
       <c r="AK82" s="10"/>
       <c r="AL82" s="10"/>
     </row>
-    <row r="83" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A83" s="2"/>
       <c r="B83" s="2"/>
       <c r="C83" s="2"/>
@@ -4037,7 +4037,7 @@
       <c r="AK83" s="10"/>
       <c r="AL83" s="10"/>
     </row>
-    <row r="84" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A84" s="2"/>
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
@@ -4077,7 +4077,7 @@
       <c r="AK84" s="10"/>
       <c r="AL84" s="10"/>
     </row>
-    <row r="85" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A85" s="2"/>
       <c r="B85" s="4"/>
       <c r="C85" s="2"/>
@@ -4117,7 +4117,7 @@
       <c r="AK85" s="10"/>
       <c r="AL85" s="10"/>
     </row>
-    <row r="86" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A86" s="2"/>
       <c r="B86" s="2"/>
       <c r="C86" s="2"/>
@@ -4157,7 +4157,7 @@
       <c r="AK86" s="10"/>
       <c r="AL86" s="10"/>
     </row>
-    <row r="87" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A87" s="2"/>
       <c r="B87" s="2"/>
       <c r="C87" s="2"/>
@@ -4197,7 +4197,7 @@
       <c r="AK87" s="10"/>
       <c r="AL87" s="10"/>
     </row>
-    <row r="88" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A88" s="2"/>
       <c r="B88" s="2"/>
       <c r="C88" s="2"/>
@@ -4237,7 +4237,7 @@
       <c r="AK88" s="10"/>
       <c r="AL88" s="10"/>
     </row>
-    <row r="89" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A89" s="2"/>
       <c r="B89" s="4"/>
       <c r="C89" s="2"/>
@@ -4277,7 +4277,7 @@
       <c r="AK89" s="10"/>
       <c r="AL89" s="10"/>
     </row>
-    <row r="90" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A90" s="2"/>
       <c r="B90" s="2"/>
       <c r="C90" s="2"/>
@@ -4317,7 +4317,7 @@
       <c r="AK90" s="10"/>
       <c r="AL90" s="10"/>
     </row>
-    <row r="91" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A91" s="2"/>
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
@@ -4357,7 +4357,7 @@
       <c r="AK91" s="10"/>
       <c r="AL91" s="10"/>
     </row>
-    <row r="92" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A92" s="2"/>
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
@@ -4397,7 +4397,7 @@
       <c r="AK92" s="10"/>
       <c r="AL92" s="10"/>
     </row>
-    <row r="93" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A93" s="2"/>
       <c r="B93" s="4"/>
       <c r="C93" s="2"/>
@@ -4437,7 +4437,7 @@
       <c r="AK93" s="10"/>
       <c r="AL93" s="10"/>
     </row>
-    <row r="94" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A94" s="2"/>
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
@@ -4477,7 +4477,7 @@
       <c r="AK94" s="10"/>
       <c r="AL94" s="10"/>
     </row>
-    <row r="95" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A95" s="2"/>
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
@@ -4517,7 +4517,7 @@
       <c r="AK95" s="10"/>
       <c r="AL95" s="10"/>
     </row>
-    <row r="96" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A96" s="2"/>
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
@@ -4557,7 +4557,7 @@
       <c r="AK96" s="10"/>
       <c r="AL96" s="10"/>
     </row>
-    <row r="97" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A97" s="2"/>
       <c r="B97" s="4"/>
       <c r="C97" s="2"/>
@@ -4597,7 +4597,7 @@
       <c r="AK97" s="10"/>
       <c r="AL97" s="10"/>
     </row>
-    <row r="98" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A98" s="2"/>
       <c r="B98" s="2"/>
       <c r="C98" s="2"/>
@@ -4637,7 +4637,7 @@
       <c r="AK98" s="10"/>
       <c r="AL98" s="10"/>
     </row>
-    <row r="99" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A99" s="2"/>
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
@@ -4677,7 +4677,7 @@
       <c r="AK99" s="10"/>
       <c r="AL99" s="10"/>
     </row>
-    <row r="100" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A100" s="2"/>
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
@@ -4717,7 +4717,7 @@
       <c r="AK100" s="10"/>
       <c r="AL100" s="10"/>
     </row>
-    <row r="101" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A101" s="2"/>
       <c r="B101" s="4"/>
       <c r="C101" s="2"/>
@@ -4757,7 +4757,7 @@
       <c r="AK101" s="10"/>
       <c r="AL101" s="10"/>
     </row>
-    <row r="102" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A102" s="2"/>
       <c r="B102" s="2"/>
       <c r="C102" s="2"/>
@@ -4797,7 +4797,7 @@
       <c r="AK102" s="10"/>
       <c r="AL102" s="10"/>
     </row>
-    <row r="103" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A103" s="2"/>
       <c r="B103" s="2"/>
       <c r="C103" s="2"/>
@@ -4837,7 +4837,7 @@
       <c r="AK103" s="10"/>
       <c r="AL103" s="10"/>
     </row>
-    <row r="104" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A104" s="2"/>
       <c r="B104" s="2"/>
       <c r="C104" s="2"/>
@@ -4877,7 +4877,7 @@
       <c r="AK104" s="10"/>
       <c r="AL104" s="10"/>
     </row>
-    <row r="105" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A105" s="2"/>
       <c r="B105" s="4"/>
       <c r="C105" s="2"/>
@@ -4917,7 +4917,7 @@
       <c r="AK105" s="10"/>
       <c r="AL105" s="10"/>
     </row>
-    <row r="106" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A106" s="2"/>
       <c r="B106" s="2"/>
       <c r="C106" s="2"/>
@@ -4957,7 +4957,7 @@
       <c r="AK106" s="10"/>
       <c r="AL106" s="10"/>
     </row>
-    <row r="107" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A107" s="2"/>
       <c r="B107" s="2"/>
       <c r="C107" s="2"/>
@@ -4997,7 +4997,7 @@
       <c r="AK107" s="10"/>
       <c r="AL107" s="10"/>
     </row>
-    <row r="108" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A108" s="2"/>
       <c r="B108" s="2"/>
       <c r="C108" s="2"/>
@@ -5037,7 +5037,7 @@
       <c r="AK108" s="10"/>
       <c r="AL108" s="10"/>
     </row>
-    <row r="109" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A109" s="2"/>
       <c r="B109" s="4"/>
       <c r="C109" s="2"/>
@@ -5077,7 +5077,7 @@
       <c r="AK109" s="10"/>
       <c r="AL109" s="10"/>
     </row>
-    <row r="110" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A110" s="2"/>
       <c r="B110" s="2"/>
       <c r="C110" s="2"/>
@@ -5117,7 +5117,7 @@
       <c r="AK110" s="10"/>
       <c r="AL110" s="10"/>
     </row>
-    <row r="111" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A111" s="2"/>
       <c r="B111" s="2"/>
       <c r="C111" s="2"/>
@@ -5157,7 +5157,7 @@
       <c r="AK111" s="10"/>
       <c r="AL111" s="10"/>
     </row>
-    <row r="112" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A112" s="2"/>
       <c r="B112" s="2"/>
       <c r="C112" s="2"/>
@@ -5197,7 +5197,7 @@
       <c r="AK112" s="10"/>
       <c r="AL112" s="10"/>
     </row>
-    <row r="113" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A113" s="2"/>
       <c r="B113" s="4"/>
       <c r="C113" s="2"/>
@@ -5237,7 +5237,7 @@
       <c r="AK113" s="10"/>
       <c r="AL113" s="10"/>
     </row>
-    <row r="114" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A114" s="2"/>
       <c r="B114" s="2"/>
       <c r="C114" s="2"/>
@@ -5277,7 +5277,7 @@
       <c r="AK114" s="10"/>
       <c r="AL114" s="10"/>
     </row>
-    <row r="115" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A115" s="2"/>
       <c r="B115" s="2"/>
       <c r="C115" s="2"/>
@@ -5317,7 +5317,7 @@
       <c r="AK115" s="10"/>
       <c r="AL115" s="10"/>
     </row>
-    <row r="116" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A116" s="2"/>
       <c r="B116" s="2"/>
       <c r="C116" s="2"/>
@@ -5357,7 +5357,7 @@
       <c r="AK116" s="10"/>
       <c r="AL116" s="10"/>
     </row>
-    <row r="117" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A117" s="2"/>
       <c r="B117" s="4"/>
       <c r="C117" s="2"/>
@@ -5397,7 +5397,7 @@
       <c r="AK117" s="10"/>
       <c r="AL117" s="10"/>
     </row>
-    <row r="118" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A118" s="2"/>
       <c r="B118" s="2"/>
       <c r="C118" s="2"/>
@@ -5437,7 +5437,7 @@
       <c r="AK118" s="10"/>
       <c r="AL118" s="10"/>
     </row>
-    <row r="119" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A119" s="2"/>
       <c r="B119" s="2"/>
       <c r="C119" s="2"/>
@@ -5477,7 +5477,7 @@
       <c r="AK119" s="10"/>
       <c r="AL119" s="10"/>
     </row>
-    <row r="120" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A120" s="2"/>
       <c r="B120" s="2"/>
       <c r="C120" s="2"/>
@@ -5517,7 +5517,7 @@
       <c r="AK120" s="10"/>
       <c r="AL120" s="10"/>
     </row>
-    <row r="121" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A121" s="2"/>
       <c r="B121" s="4"/>
       <c r="C121" s="2"/>
@@ -5557,7 +5557,7 @@
       <c r="AK121" s="10"/>
       <c r="AL121" s="10"/>
     </row>
-    <row r="122" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A122" s="2"/>
       <c r="B122" s="2"/>
       <c r="C122" s="2"/>
@@ -5597,7 +5597,7 @@
       <c r="AK122" s="10"/>
       <c r="AL122" s="10"/>
     </row>
-    <row r="123" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A123" s="2"/>
       <c r="B123" s="2"/>
       <c r="C123" s="2"/>
@@ -5637,7 +5637,7 @@
       <c r="AK123" s="10"/>
       <c r="AL123" s="10"/>
     </row>
-    <row r="124" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A124" s="2"/>
       <c r="B124" s="2"/>
       <c r="C124" s="2"/>
@@ -5677,7 +5677,7 @@
       <c r="AK124" s="10"/>
       <c r="AL124" s="10"/>
     </row>
-    <row r="125" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A125" s="2"/>
       <c r="B125" s="4"/>
       <c r="C125" s="2"/>
@@ -5717,7 +5717,7 @@
       <c r="AK125" s="10"/>
       <c r="AL125" s="10"/>
     </row>
-    <row r="126" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A126" s="2"/>
       <c r="B126" s="2"/>
       <c r="C126" s="2"/>
@@ -5757,7 +5757,7 @@
       <c r="AK126" s="10"/>
       <c r="AL126" s="10"/>
     </row>
-    <row r="127" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A127" s="2"/>
       <c r="B127" s="2"/>
       <c r="C127" s="2"/>
@@ -5797,7 +5797,7 @@
       <c r="AK127" s="10"/>
       <c r="AL127" s="10"/>
     </row>
-    <row r="128" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A128" s="2"/>
       <c r="B128" s="2"/>
       <c r="C128" s="2"/>
@@ -5837,7 +5837,7 @@
       <c r="AK128" s="10"/>
       <c r="AL128" s="10"/>
     </row>
-    <row r="129" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A129" s="2"/>
       <c r="B129" s="4"/>
       <c r="C129" s="2"/>
@@ -5877,7 +5877,7 @@
       <c r="AK129" s="10"/>
       <c r="AL129" s="10"/>
     </row>
-    <row r="130" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A130" s="2"/>
       <c r="B130" s="2"/>
       <c r="C130" s="2"/>
@@ -5917,7 +5917,7 @@
       <c r="AK130" s="10"/>
       <c r="AL130" s="10"/>
     </row>
-    <row r="131" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A131" s="2"/>
       <c r="B131" s="2"/>
       <c r="C131" s="2"/>
@@ -5957,7 +5957,7 @@
       <c r="AK131" s="10"/>
       <c r="AL131" s="10"/>
     </row>
-    <row r="132" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A132" s="2"/>
       <c r="B132" s="2"/>
       <c r="C132" s="2"/>
@@ -5997,7 +5997,7 @@
       <c r="AK132" s="10"/>
       <c r="AL132" s="10"/>
     </row>
-    <row r="133" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A133" s="2"/>
       <c r="B133" s="4"/>
       <c r="C133" s="2"/>
@@ -6037,7 +6037,7 @@
       <c r="AK133" s="10"/>
       <c r="AL133" s="10"/>
     </row>
-    <row r="134" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A134" s="2"/>
       <c r="B134" s="2"/>
       <c r="C134" s="2"/>
@@ -6077,7 +6077,7 @@
       <c r="AK134" s="10"/>
       <c r="AL134" s="10"/>
     </row>
-    <row r="135" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A135" s="2"/>
       <c r="B135" s="2"/>
       <c r="C135" s="2"/>
@@ -6117,7 +6117,7 @@
       <c r="AK135" s="10"/>
       <c r="AL135" s="10"/>
     </row>
-    <row r="136" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A136" s="2"/>
       <c r="B136" s="2"/>
       <c r="C136" s="2"/>
@@ -6157,7 +6157,7 @@
       <c r="AK136" s="10"/>
       <c r="AL136" s="10"/>
     </row>
-    <row r="137" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A137" s="2"/>
       <c r="B137" s="4"/>
       <c r="C137" s="2"/>
@@ -6197,7 +6197,7 @@
       <c r="AK137" s="10"/>
       <c r="AL137" s="10"/>
     </row>
-    <row r="138" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A138" s="2"/>
       <c r="B138" s="2"/>
       <c r="C138" s="2"/>
@@ -6237,7 +6237,7 @@
       <c r="AK138" s="10"/>
       <c r="AL138" s="10"/>
     </row>
-    <row r="139" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A139" s="2"/>
       <c r="B139" s="2"/>
       <c r="C139" s="2"/>
@@ -6277,7 +6277,7 @@
       <c r="AK139" s="10"/>
       <c r="AL139" s="10"/>
     </row>
-    <row r="140" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A140" s="2"/>
       <c r="B140" s="2"/>
       <c r="C140" s="2"/>
@@ -6317,7 +6317,7 @@
       <c r="AK140" s="10"/>
       <c r="AL140" s="10"/>
     </row>
-    <row r="141" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A141" s="2"/>
       <c r="B141" s="4"/>
       <c r="C141" s="2"/>
@@ -6357,7 +6357,7 @@
       <c r="AK141" s="10"/>
       <c r="AL141" s="10"/>
     </row>
-    <row r="142" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A142" s="2"/>
       <c r="B142" s="2"/>
       <c r="C142" s="2"/>
@@ -6397,7 +6397,7 @@
       <c r="AK142" s="10"/>
       <c r="AL142" s="10"/>
     </row>
-    <row r="143" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A143" s="2"/>
       <c r="B143" s="2"/>
       <c r="C143" s="2"/>
@@ -6437,7 +6437,7 @@
       <c r="AK143" s="10"/>
       <c r="AL143" s="10"/>
     </row>
-    <row r="144" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A144" s="2"/>
       <c r="B144" s="2"/>
       <c r="C144" s="2"/>
@@ -6477,7 +6477,7 @@
       <c r="AK144" s="10"/>
       <c r="AL144" s="10"/>
     </row>
-    <row r="145" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A145" s="2"/>
       <c r="B145" s="4"/>
       <c r="C145" s="2"/>
@@ -6517,7 +6517,7 @@
       <c r="AK145" s="10"/>
       <c r="AL145" s="10"/>
     </row>
-    <row r="146" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A146" s="2"/>
       <c r="B146" s="2"/>
       <c r="C146" s="2"/>
@@ -6557,7 +6557,7 @@
       <c r="AK146" s="10"/>
       <c r="AL146" s="10"/>
     </row>
-    <row r="147" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A147" s="2"/>
       <c r="B147" s="2"/>
       <c r="C147" s="2"/>
@@ -6597,7 +6597,7 @@
       <c r="AK147" s="10"/>
       <c r="AL147" s="10"/>
     </row>
-    <row r="148" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A148" s="2"/>
       <c r="B148" s="2"/>
       <c r="C148" s="2"/>
@@ -6637,7 +6637,7 @@
       <c r="AK148" s="10"/>
       <c r="AL148" s="10"/>
     </row>
-    <row r="149" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A149" s="2"/>
       <c r="B149" s="4"/>
       <c r="C149" s="2"/>
@@ -6677,7 +6677,7 @@
       <c r="AK149" s="10"/>
       <c r="AL149" s="10"/>
     </row>
-    <row r="150" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A150" s="2"/>
       <c r="B150" s="2"/>
       <c r="C150" s="2"/>
@@ -6717,7 +6717,7 @@
       <c r="AK150" s="10"/>
       <c r="AL150" s="10"/>
     </row>
-    <row r="151" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A151" s="2"/>
       <c r="B151" s="2"/>
       <c r="C151" s="2"/>
@@ -6757,7 +6757,7 @@
       <c r="AK151" s="10"/>
       <c r="AL151" s="10"/>
     </row>
-    <row r="152" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A152" s="2"/>
       <c r="B152" s="2"/>
       <c r="C152" s="2"/>
@@ -6797,7 +6797,7 @@
       <c r="AK152" s="10"/>
       <c r="AL152" s="10"/>
     </row>
-    <row r="153" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A153" s="2"/>
       <c r="B153" s="4"/>
       <c r="C153" s="2"/>
@@ -6837,7 +6837,7 @@
       <c r="AK153" s="10"/>
       <c r="AL153" s="10"/>
     </row>
-    <row r="154" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A154" s="2"/>
       <c r="B154" s="2"/>
       <c r="C154" s="2"/>
@@ -6877,7 +6877,7 @@
       <c r="AK154" s="10"/>
       <c r="AL154" s="10"/>
     </row>
-    <row r="155" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A155" s="2"/>
       <c r="B155" s="2"/>
       <c r="C155" s="2"/>
@@ -6917,7 +6917,7 @@
       <c r="AK155" s="10"/>
       <c r="AL155" s="10"/>
     </row>
-    <row r="156" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A156" s="2"/>
       <c r="B156" s="2"/>
       <c r="C156" s="2"/>
@@ -6957,7 +6957,7 @@
       <c r="AK156" s="10"/>
       <c r="AL156" s="10"/>
     </row>
-    <row r="157" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A157" s="2"/>
       <c r="B157" s="4"/>
       <c r="C157" s="2"/>
@@ -6997,7 +6997,7 @@
       <c r="AK157" s="10"/>
       <c r="AL157" s="10"/>
     </row>
-    <row r="158" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A158" s="2"/>
       <c r="B158" s="2"/>
       <c r="C158" s="2"/>
@@ -7037,7 +7037,7 @@
       <c r="AK158" s="10"/>
       <c r="AL158" s="10"/>
     </row>
-    <row r="159" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A159" s="2"/>
       <c r="B159" s="2"/>
       <c r="C159" s="2"/>
@@ -7077,7 +7077,7 @@
       <c r="AK159" s="10"/>
       <c r="AL159" s="10"/>
     </row>
-    <row r="160" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A160" s="2"/>
       <c r="B160" s="2"/>
       <c r="C160" s="2"/>
@@ -7117,7 +7117,7 @@
       <c r="AK160" s="10"/>
       <c r="AL160" s="10"/>
     </row>
-    <row r="161" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A161" s="2"/>
       <c r="B161" s="4"/>
       <c r="C161" s="2"/>
@@ -7157,7 +7157,7 @@
       <c r="AK161" s="10"/>
       <c r="AL161" s="10"/>
     </row>
-    <row r="162" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A162" s="2"/>
       <c r="B162" s="2"/>
       <c r="C162" s="2"/>
@@ -7197,7 +7197,7 @@
       <c r="AK162" s="10"/>
       <c r="AL162" s="10"/>
     </row>
-    <row r="163" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A163" s="2"/>
       <c r="B163" s="2"/>
       <c r="C163" s="2"/>
@@ -7237,7 +7237,7 @@
       <c r="AK163" s="10"/>
       <c r="AL163" s="10"/>
     </row>
-    <row r="164" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A164" s="2"/>
       <c r="B164" s="2"/>
       <c r="C164" s="2"/>
@@ -7277,7 +7277,7 @@
       <c r="AK164" s="10"/>
       <c r="AL164" s="10"/>
     </row>
-    <row r="165" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A165" s="2"/>
       <c r="B165" s="4"/>
       <c r="C165" s="2"/>
@@ -7317,7 +7317,7 @@
       <c r="AK165" s="10"/>
       <c r="AL165" s="10"/>
     </row>
-    <row r="166" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A166" s="2"/>
       <c r="B166" s="2"/>
       <c r="C166" s="2"/>
@@ -7357,7 +7357,7 @@
       <c r="AK166" s="10"/>
       <c r="AL166" s="10"/>
     </row>
-    <row r="167" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A167" s="2"/>
       <c r="B167" s="2"/>
       <c r="C167" s="2"/>
@@ -7397,7 +7397,7 @@
       <c r="AK167" s="10"/>
       <c r="AL167" s="10"/>
     </row>
-    <row r="168" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A168" s="2"/>
       <c r="B168" s="2"/>
       <c r="C168" s="2"/>
@@ -7437,7 +7437,7 @@
       <c r="AK168" s="10"/>
       <c r="AL168" s="10"/>
     </row>
-    <row r="169" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A169" s="2"/>
       <c r="B169" s="4"/>
       <c r="C169" s="2"/>
@@ -7477,7 +7477,7 @@
       <c r="AK169" s="10"/>
       <c r="AL169" s="10"/>
     </row>
-    <row r="170" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A170" s="2"/>
       <c r="B170" s="2"/>
       <c r="C170" s="2"/>
@@ -7517,7 +7517,7 @@
       <c r="AK170" s="10"/>
       <c r="AL170" s="10"/>
     </row>
-    <row r="171" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A171" s="2"/>
       <c r="B171" s="2"/>
       <c r="C171" s="2"/>
@@ -7557,7 +7557,7 @@
       <c r="AK171" s="10"/>
       <c r="AL171" s="10"/>
     </row>
-    <row r="172" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A172" s="2"/>
       <c r="B172" s="2"/>
       <c r="C172" s="2"/>
@@ -7597,7 +7597,7 @@
       <c r="AK172" s="10"/>
       <c r="AL172" s="10"/>
     </row>
-    <row r="173" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A173" s="2"/>
       <c r="B173" s="4"/>
       <c r="C173" s="2"/>
@@ -7637,7 +7637,7 @@
       <c r="AK173" s="10"/>
       <c r="AL173" s="10"/>
     </row>
-    <row r="174" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A174" s="2"/>
       <c r="B174" s="2"/>
       <c r="C174" s="2"/>
@@ -7677,7 +7677,7 @@
       <c r="AK174" s="10"/>
       <c r="AL174" s="10"/>
     </row>
-    <row r="175" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A175" s="2"/>
       <c r="B175" s="2"/>
       <c r="C175" s="2"/>
@@ -7717,7 +7717,7 @@
       <c r="AK175" s="10"/>
       <c r="AL175" s="10"/>
     </row>
-    <row r="176" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A176" s="2"/>
       <c r="B176" s="2"/>
       <c r="C176" s="2"/>
@@ -7757,7 +7757,7 @@
       <c r="AK176" s="10"/>
       <c r="AL176" s="10"/>
     </row>
-    <row r="177" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A177" s="2"/>
       <c r="B177" s="4"/>
       <c r="C177" s="2"/>
@@ -7797,7 +7797,7 @@
       <c r="AK177" s="10"/>
       <c r="AL177" s="10"/>
     </row>
-    <row r="178" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A178" s="2"/>
       <c r="B178" s="2"/>
       <c r="C178" s="2"/>
@@ -7837,7 +7837,7 @@
       <c r="AK178" s="10"/>
       <c r="AL178" s="10"/>
     </row>
-    <row r="179" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A179" s="2"/>
       <c r="B179" s="2"/>
       <c r="C179" s="2"/>
@@ -7877,7 +7877,7 @@
       <c r="AK179" s="10"/>
       <c r="AL179" s="10"/>
     </row>
-    <row r="180" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A180" s="2"/>
       <c r="B180" s="2"/>
       <c r="C180" s="2"/>
@@ -7917,7 +7917,7 @@
       <c r="AK180" s="10"/>
       <c r="AL180" s="10"/>
     </row>
-    <row r="181" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A181" s="2"/>
       <c r="B181" s="4"/>
       <c r="C181" s="2"/>
@@ -7957,7 +7957,7 @@
       <c r="AK181" s="10"/>
       <c r="AL181" s="10"/>
     </row>
-    <row r="182" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A182" s="2"/>
       <c r="B182" s="2"/>
       <c r="C182" s="2"/>
@@ -7997,7 +7997,7 @@
       <c r="AK182" s="10"/>
       <c r="AL182" s="10"/>
     </row>
-    <row r="183" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A183" s="2"/>
       <c r="B183" s="2"/>
       <c r="C183" s="2"/>
@@ -8037,7 +8037,7 @@
       <c r="AK183" s="10"/>
       <c r="AL183" s="10"/>
     </row>
-    <row r="184" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A184" s="2"/>
       <c r="B184" s="2"/>
       <c r="C184" s="2"/>
@@ -8077,7 +8077,7 @@
       <c r="AK184" s="10"/>
       <c r="AL184" s="10"/>
     </row>
-    <row r="185" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A185" s="2"/>
       <c r="B185" s="4"/>
       <c r="C185" s="2"/>
@@ -8117,7 +8117,7 @@
       <c r="AK185" s="10"/>
       <c r="AL185" s="10"/>
     </row>
-    <row r="186" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A186" s="2"/>
       <c r="B186" s="2"/>
       <c r="C186" s="2"/>
@@ -8157,7 +8157,7 @@
       <c r="AK186" s="10"/>
       <c r="AL186" s="10"/>
     </row>
-    <row r="187" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A187" s="2"/>
       <c r="B187" s="2"/>
       <c r="C187" s="2"/>
@@ -8197,7 +8197,7 @@
       <c r="AK187" s="10"/>
       <c r="AL187" s="10"/>
     </row>
-    <row r="188" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A188" s="2"/>
       <c r="B188" s="2"/>
       <c r="C188" s="2"/>
@@ -8237,7 +8237,7 @@
       <c r="AK188" s="10"/>
       <c r="AL188" s="10"/>
     </row>
-    <row r="189" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A189" s="2"/>
       <c r="B189" s="4"/>
       <c r="C189" s="2"/>
@@ -8277,7 +8277,7 @@
       <c r="AK189" s="10"/>
       <c r="AL189" s="10"/>
     </row>
-    <row r="190" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A190" s="2"/>
       <c r="B190" s="2"/>
       <c r="C190" s="2"/>
@@ -8317,7 +8317,7 @@
       <c r="AK190" s="10"/>
       <c r="AL190" s="10"/>
     </row>
-    <row r="191" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A191" s="2"/>
       <c r="B191" s="2"/>
       <c r="C191" s="2"/>
@@ -8357,7 +8357,7 @@
       <c r="AK191" s="10"/>
       <c r="AL191" s="10"/>
     </row>
-    <row r="192" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A192" s="2"/>
       <c r="B192" s="2"/>
       <c r="C192" s="2"/>
@@ -8397,7 +8397,7 @@
       <c r="AK192" s="10"/>
       <c r="AL192" s="10"/>
     </row>
-    <row r="193" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A193" s="2"/>
       <c r="B193" s="4"/>
       <c r="C193" s="2"/>
@@ -8437,7 +8437,7 @@
       <c r="AK193" s="10"/>
       <c r="AL193" s="10"/>
     </row>
-    <row r="194" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A194" s="2"/>
       <c r="B194" s="2"/>
       <c r="C194" s="2"/>
@@ -8477,7 +8477,7 @@
       <c r="AK194" s="10"/>
       <c r="AL194" s="10"/>
     </row>
-    <row r="195" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A195" s="2"/>
       <c r="B195" s="2"/>
       <c r="C195" s="2"/>
@@ -8517,7 +8517,7 @@
       <c r="AK195" s="10"/>
       <c r="AL195" s="10"/>
     </row>
-    <row r="196" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A196" s="2"/>
       <c r="B196" s="2"/>
       <c r="C196" s="2"/>
@@ -8557,7 +8557,7 @@
       <c r="AK196" s="10"/>
       <c r="AL196" s="10"/>
     </row>
-    <row r="197" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A197" s="2"/>
       <c r="B197" s="4"/>
       <c r="C197" s="2"/>
@@ -8597,7 +8597,7 @@
       <c r="AK197" s="10"/>
       <c r="AL197" s="10"/>
     </row>
-    <row r="198" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A198" s="2"/>
       <c r="B198" s="2"/>
       <c r="C198" s="2"/>
@@ -8637,7 +8637,7 @@
       <c r="AK198" s="10"/>
       <c r="AL198" s="10"/>
     </row>
-    <row r="199" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A199" s="2"/>
       <c r="B199" s="2"/>
       <c r="C199" s="2"/>
@@ -8677,7 +8677,7 @@
       <c r="AK199" s="10"/>
       <c r="AL199" s="10"/>
     </row>
-    <row r="200" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A200" s="2"/>
       <c r="B200" s="2"/>
       <c r="C200" s="2"/>
@@ -8717,7 +8717,7 @@
       <c r="AK200" s="10"/>
       <c r="AL200" s="10"/>
     </row>
-    <row r="201" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A201" s="2"/>
       <c r="B201" s="4"/>
       <c r="C201" s="2"/>
@@ -8757,7 +8757,7 @@
       <c r="AK201" s="10"/>
       <c r="AL201" s="10"/>
     </row>
-    <row r="202" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A202" s="2"/>
       <c r="B202" s="2"/>
       <c r="C202" s="2"/>
@@ -8797,7 +8797,7 @@
       <c r="AK202" s="10"/>
       <c r="AL202" s="10"/>
     </row>
-    <row r="203" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A203" s="2"/>
       <c r="B203" s="2"/>
       <c r="C203" s="2"/>
@@ -8837,7 +8837,7 @@
       <c r="AK203" s="10"/>
       <c r="AL203" s="10"/>
     </row>
-    <row r="204" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A204" s="2"/>
       <c r="B204" s="2"/>
       <c r="C204" s="2"/>
@@ -8877,7 +8877,7 @@
       <c r="AK204" s="10"/>
       <c r="AL204" s="10"/>
     </row>
-    <row r="205" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A205" s="2"/>
       <c r="B205" s="4"/>
       <c r="C205" s="2"/>
@@ -8917,7 +8917,7 @@
       <c r="AK205" s="10"/>
       <c r="AL205" s="10"/>
     </row>
-    <row r="206" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A206" s="2"/>
       <c r="B206" s="2"/>
       <c r="C206" s="2"/>
@@ -8957,7 +8957,7 @@
       <c r="AK206" s="10"/>
       <c r="AL206" s="10"/>
     </row>
-    <row r="207" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A207" s="2"/>
       <c r="B207" s="2"/>
       <c r="C207" s="2"/>
@@ -8997,7 +8997,7 @@
       <c r="AK207" s="10"/>
       <c r="AL207" s="10"/>
     </row>
-    <row r="208" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A208" s="2"/>
       <c r="B208" s="2"/>
       <c r="C208" s="2"/>
@@ -9037,7 +9037,7 @@
       <c r="AK208" s="10"/>
       <c r="AL208" s="10"/>
     </row>
-    <row r="209" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A209" s="2"/>
       <c r="B209" s="4"/>
       <c r="C209" s="2"/>
@@ -9077,7 +9077,7 @@
       <c r="AK209" s="10"/>
       <c r="AL209" s="10"/>
     </row>
-    <row r="210" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A210" s="2"/>
       <c r="B210" s="2"/>
       <c r="C210" s="2"/>
@@ -9117,7 +9117,7 @@
       <c r="AK210" s="10"/>
       <c r="AL210" s="10"/>
     </row>
-    <row r="211" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A211" s="2"/>
       <c r="B211" s="2"/>
       <c r="C211" s="2"/>
@@ -9157,7 +9157,7 @@
       <c r="AK211" s="10"/>
       <c r="AL211" s="10"/>
     </row>
-    <row r="212" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A212" s="2"/>
       <c r="B212" s="2"/>
       <c r="C212" s="2"/>
@@ -9197,7 +9197,7 @@
       <c r="AK212" s="10"/>
       <c r="AL212" s="10"/>
     </row>
-    <row r="213" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A213" s="2"/>
       <c r="B213" s="4"/>
       <c r="C213" s="2"/>
@@ -9237,7 +9237,7 @@
       <c r="AK213" s="10"/>
       <c r="AL213" s="10"/>
     </row>
-    <row r="214" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A214" s="2"/>
       <c r="B214" s="2"/>
       <c r="C214" s="2"/>
@@ -9277,7 +9277,7 @@
       <c r="AK214" s="10"/>
       <c r="AL214" s="10"/>
     </row>
-    <row r="215" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A215" s="2"/>
       <c r="B215" s="2"/>
       <c r="C215" s="2"/>
@@ -9317,7 +9317,7 @@
       <c r="AK215" s="10"/>
       <c r="AL215" s="10"/>
     </row>
-    <row r="216" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A216" s="2"/>
       <c r="B216" s="2"/>
       <c r="C216" s="2"/>
@@ -9357,7 +9357,7 @@
       <c r="AK216" s="10"/>
       <c r="AL216" s="10"/>
     </row>
-    <row r="217" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A217" s="2"/>
       <c r="B217" s="4"/>
       <c r="C217" s="2"/>
@@ -9397,7 +9397,7 @@
       <c r="AK217" s="10"/>
       <c r="AL217" s="10"/>
     </row>
-    <row r="218" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A218" s="2"/>
       <c r="B218" s="2"/>
       <c r="C218" s="2"/>
@@ -9437,7 +9437,7 @@
       <c r="AK218" s="10"/>
       <c r="AL218" s="10"/>
     </row>
-    <row r="219" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A219" s="2"/>
       <c r="B219" s="2"/>
       <c r="C219" s="2"/>
@@ -9477,7 +9477,7 @@
       <c r="AK219" s="10"/>
       <c r="AL219" s="10"/>
     </row>
-    <row r="220" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A220" s="2"/>
       <c r="B220" s="2"/>
       <c r="C220" s="2"/>
@@ -9517,7 +9517,7 @@
       <c r="AK220" s="10"/>
       <c r="AL220" s="10"/>
     </row>
-    <row r="221" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A221" s="2"/>
       <c r="B221" s="4"/>
       <c r="C221" s="2"/>
@@ -9557,7 +9557,7 @@
       <c r="AK221" s="10"/>
       <c r="AL221" s="10"/>
     </row>
-    <row r="222" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A222" s="2"/>
       <c r="B222" s="2"/>
       <c r="C222" s="2"/>
@@ -9597,7 +9597,7 @@
       <c r="AK222" s="10"/>
       <c r="AL222" s="10"/>
     </row>
-    <row r="223" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A223" s="2"/>
       <c r="B223" s="2"/>
       <c r="C223" s="2"/>
@@ -9637,7 +9637,7 @@
       <c r="AK223" s="10"/>
       <c r="AL223" s="10"/>
     </row>
-    <row r="224" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A224" s="2"/>
       <c r="B224" s="2"/>
       <c r="C224" s="2"/>
@@ -9677,7 +9677,7 @@
       <c r="AK224" s="10"/>
       <c r="AL224" s="10"/>
     </row>
-    <row r="225" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A225" s="2"/>
       <c r="B225" s="4"/>
       <c r="C225" s="2"/>
@@ -9717,7 +9717,7 @@
       <c r="AK225" s="10"/>
       <c r="AL225" s="10"/>
     </row>
-    <row r="226" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A226" s="2"/>
       <c r="B226" s="2"/>
       <c r="C226" s="2"/>
@@ -9757,7 +9757,7 @@
       <c r="AK226" s="10"/>
       <c r="AL226" s="10"/>
     </row>
-    <row r="227" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A227" s="2"/>
       <c r="B227" s="2"/>
       <c r="C227" s="2"/>
@@ -9797,7 +9797,7 @@
       <c r="AK227" s="10"/>
       <c r="AL227" s="10"/>
     </row>
-    <row r="228" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A228" s="2"/>
       <c r="B228" s="2"/>
       <c r="C228" s="2"/>
@@ -9837,7 +9837,7 @@
       <c r="AK228" s="10"/>
       <c r="AL228" s="10"/>
     </row>
-    <row r="229" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A229" s="2"/>
       <c r="B229" s="4"/>
       <c r="C229" s="2"/>
@@ -9877,7 +9877,7 @@
       <c r="AK229" s="10"/>
       <c r="AL229" s="10"/>
     </row>
-    <row r="230" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A230" s="2"/>
       <c r="B230" s="2"/>
       <c r="C230" s="2"/>
@@ -9917,7 +9917,7 @@
       <c r="AK230" s="10"/>
       <c r="AL230" s="10"/>
     </row>
-    <row r="231" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A231" s="2"/>
       <c r="B231" s="2"/>
       <c r="C231" s="2"/>
@@ -9957,7 +9957,7 @@
       <c r="AK231" s="10"/>
       <c r="AL231" s="10"/>
     </row>
-    <row r="232" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A232" s="2"/>
       <c r="B232" s="2"/>
       <c r="C232" s="2"/>
@@ -9997,7 +9997,7 @@
       <c r="AK232" s="10"/>
       <c r="AL232" s="10"/>
     </row>
-    <row r="233" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A233" s="2"/>
       <c r="B233" s="4"/>
       <c r="C233" s="2"/>
@@ -10037,7 +10037,7 @@
       <c r="AK233" s="10"/>
       <c r="AL233" s="10"/>
     </row>
-    <row r="234" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A234" s="2"/>
       <c r="B234" s="2"/>
       <c r="C234" s="2"/>
@@ -10077,7 +10077,7 @@
       <c r="AK234" s="10"/>
       <c r="AL234" s="10"/>
     </row>
-    <row r="235" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A235" s="2"/>
       <c r="B235" s="2"/>
       <c r="C235" s="2"/>
@@ -10117,7 +10117,7 @@
       <c r="AK235" s="10"/>
       <c r="AL235" s="10"/>
     </row>
-    <row r="236" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A236" s="2"/>
       <c r="B236" s="2"/>
       <c r="C236" s="2"/>
@@ -10157,7 +10157,7 @@
       <c r="AK236" s="10"/>
       <c r="AL236" s="10"/>
     </row>
-    <row r="237" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A237" s="2"/>
       <c r="B237" s="4"/>
       <c r="C237" s="2"/>
@@ -10197,7 +10197,7 @@
       <c r="AK237" s="10"/>
       <c r="AL237" s="10"/>
     </row>
-    <row r="238" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A238" s="2"/>
       <c r="B238" s="2"/>
       <c r="C238" s="2"/>
@@ -10237,7 +10237,7 @@
       <c r="AK238" s="10"/>
       <c r="AL238" s="10"/>
     </row>
-    <row r="239" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A239" s="2"/>
       <c r="B239" s="2"/>
       <c r="C239" s="2"/>
@@ -10277,7 +10277,7 @@
       <c r="AK239" s="10"/>
       <c r="AL239" s="10"/>
     </row>
-    <row r="240" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A240" s="2"/>
       <c r="B240" s="2"/>
       <c r="C240" s="2"/>
@@ -10317,7 +10317,7 @@
       <c r="AK240" s="10"/>
       <c r="AL240" s="10"/>
     </row>
-    <row r="241" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A241" s="2"/>
       <c r="B241" s="4"/>
       <c r="C241" s="2"/>
@@ -10357,7 +10357,7 @@
       <c r="AK241" s="10"/>
       <c r="AL241" s="10"/>
     </row>
-    <row r="242" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A242" s="2"/>
       <c r="B242" s="2"/>
       <c r="C242" s="2"/>
@@ -10397,7 +10397,7 @@
       <c r="AK242" s="10"/>
       <c r="AL242" s="10"/>
     </row>
-    <row r="243" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A243" s="2"/>
       <c r="B243" s="2"/>
       <c r="C243" s="2"/>
@@ -10437,7 +10437,7 @@
       <c r="AK243" s="10"/>
       <c r="AL243" s="10"/>
     </row>
-    <row r="244" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A244" s="2"/>
       <c r="B244" s="2"/>
       <c r="C244" s="2"/>
@@ -10477,7 +10477,7 @@
       <c r="AK244" s="10"/>
       <c r="AL244" s="10"/>
     </row>
-    <row r="245" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A245" s="2"/>
       <c r="B245" s="4"/>
       <c r="C245" s="2"/>
@@ -10517,7 +10517,7 @@
       <c r="AK245" s="10"/>
       <c r="AL245" s="10"/>
     </row>
-    <row r="246" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A246" s="2"/>
       <c r="B246" s="2"/>
       <c r="C246" s="2"/>
@@ -10557,7 +10557,7 @@
       <c r="AK246" s="10"/>
       <c r="AL246" s="10"/>
     </row>
-    <row r="247" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A247" s="2"/>
       <c r="B247" s="2"/>
       <c r="C247" s="2"/>
@@ -10597,7 +10597,7 @@
       <c r="AK247" s="10"/>
       <c r="AL247" s="10"/>
     </row>
-    <row r="248" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A248" s="2"/>
       <c r="B248" s="2"/>
       <c r="C248" s="2"/>
@@ -10637,7 +10637,7 @@
       <c r="AK248" s="10"/>
       <c r="AL248" s="10"/>
     </row>
-    <row r="249" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A249" s="2"/>
       <c r="B249" s="4"/>
       <c r="C249" s="2"/>
@@ -10677,7 +10677,7 @@
       <c r="AK249" s="10"/>
       <c r="AL249" s="10"/>
     </row>
-    <row r="250" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A250" s="2"/>
       <c r="B250" s="2"/>
       <c r="C250" s="2"/>
@@ -10717,7 +10717,7 @@
       <c r="AK250" s="10"/>
       <c r="AL250" s="10"/>
     </row>
-    <row r="251" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A251" s="2"/>
       <c r="B251" s="2"/>
       <c r="C251" s="2"/>
@@ -10757,7 +10757,7 @@
       <c r="AK251" s="10"/>
       <c r="AL251" s="10"/>
     </row>
-    <row r="252" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A252" s="2"/>
       <c r="B252" s="2"/>
       <c r="C252" s="2"/>
@@ -10797,7 +10797,7 @@
       <c r="AK252" s="10"/>
       <c r="AL252" s="10"/>
     </row>
-    <row r="253" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A253" s="2"/>
       <c r="B253" s="4"/>
       <c r="C253" s="2"/>
@@ -10837,7 +10837,7 @@
       <c r="AK253" s="10"/>
       <c r="AL253" s="10"/>
     </row>
-    <row r="254" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A254" s="2"/>
       <c r="B254" s="2"/>
       <c r="C254" s="2"/>
@@ -10877,7 +10877,7 @@
       <c r="AK254" s="10"/>
       <c r="AL254" s="10"/>
     </row>
-    <row r="255" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A255" s="2"/>
       <c r="B255" s="2"/>
       <c r="C255" s="2"/>
@@ -10917,7 +10917,7 @@
       <c r="AK255" s="10"/>
       <c r="AL255" s="10"/>
     </row>
-    <row r="256" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A256" s="2"/>
       <c r="B256" s="2"/>
       <c r="C256" s="2"/>
@@ -10957,7 +10957,7 @@
       <c r="AK256" s="10"/>
       <c r="AL256" s="10"/>
     </row>
-    <row r="257" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A257" s="2"/>
       <c r="B257" s="4"/>
       <c r="C257" s="2"/>
@@ -10997,7 +10997,7 @@
       <c r="AK257" s="10"/>
       <c r="AL257" s="10"/>
     </row>
-    <row r="258" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A258" s="2"/>
       <c r="B258" s="2"/>
       <c r="C258" s="2"/>
@@ -11037,7 +11037,7 @@
       <c r="AK258" s="10"/>
       <c r="AL258" s="10"/>
     </row>
-    <row r="259" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A259" s="2"/>
       <c r="B259" s="2"/>
       <c r="C259" s="2"/>
@@ -11077,7 +11077,7 @@
       <c r="AK259" s="10"/>
       <c r="AL259" s="10"/>
     </row>
-    <row r="260" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A260" s="2"/>
       <c r="B260" s="2"/>
       <c r="C260" s="2"/>
@@ -11140,7 +11140,7 @@
       <selection activeCell="L255" sqref="L255"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -11157,7 +11157,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
Fixed template for importing farmers
</commit_message>
<xml_diff>
--- a/src/assets/farmer-import/Template_list of farmers_NEW.xlsx
+++ b/src/assets/farmer-import/Template_list of farmers_NEW.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bpaspalovski/IntellijProjects/inatrace/inatrace-fe/src/assets/farmer-import/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{657AFD19-E069-1245-8E26-B400E0E1B0AF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F39A5A1B-2F8D-C844-B767-CB25519013C2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3440" yWindow="500" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>List of farmers</t>
   </si>
@@ -145,118 +145,10 @@
     </r>
   </si>
   <si>
-    <t>A1</t>
-  </si>
-  <si>
-    <t>A2</t>
-  </si>
-  <si>
-    <t>A3</t>
-  </si>
-  <si>
-    <t>A4</t>
-  </si>
-  <si>
-    <t>A5</t>
-  </si>
-  <si>
-    <t>A6</t>
-  </si>
-  <si>
-    <t>A7</t>
-  </si>
-  <si>
-    <t>A8</t>
-  </si>
-  <si>
-    <t>A9</t>
-  </si>
-  <si>
-    <t>A10</t>
-  </si>
-  <si>
-    <t>A11</t>
-  </si>
-  <si>
-    <t>A12</t>
-  </si>
-  <si>
-    <t>A13</t>
-  </si>
-  <si>
-    <t>A14</t>
-  </si>
-  <si>
-    <t>A15</t>
-  </si>
-  <si>
-    <t>A16</t>
-  </si>
-  <si>
-    <t>A17</t>
-  </si>
-  <si>
-    <t>A18</t>
-  </si>
-  <si>
-    <t>A19</t>
-  </si>
-  <si>
-    <t>A20</t>
-  </si>
-  <si>
-    <t>A21</t>
-  </si>
-  <si>
-    <t>A22</t>
-  </si>
-  <si>
-    <t>A23</t>
-  </si>
-  <si>
-    <t>L-PT-1-1</t>
-  </si>
-  <si>
-    <t>L-PT-1-2</t>
-  </si>
-  <si>
-    <t>L-PT-2-1</t>
-  </si>
-  <si>
-    <t>L-PT-2-2</t>
-  </si>
-  <si>
-    <t>A24</t>
-  </si>
-  <si>
-    <t>A25</t>
-  </si>
-  <si>
-    <t>A26</t>
-  </si>
-  <si>
-    <t>A27</t>
-  </si>
-  <si>
-    <t>A28</t>
-  </si>
-  <si>
-    <t>A29</t>
-  </si>
-  <si>
-    <t>A30</t>
-  </si>
-  <si>
     <t>Area cultivated with coffee</t>
   </si>
   <si>
     <t>Number of coffee plants</t>
-  </si>
-  <si>
-    <t>Area cultivated with macadamia</t>
-  </si>
-  <si>
-    <t>Number of macadamia plants</t>
   </si>
 </sst>
 </file>
@@ -477,10 +369,10 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="25">
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -845,8 +737,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AN260"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U2" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="AA7" sqref="AA7"/>
+    <sheetView tabSelected="1" topLeftCell="U1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="AA2" sqref="AA2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -877,11 +769,11 @@
       <c r="Q1" s="1"/>
     </row>
     <row r="2" spans="1:40" ht="26" x14ac:dyDescent="0.25">
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
       <c r="F2" s="19"/>
       <c r="G2" s="19"/>
       <c r="H2" s="19"/>
@@ -912,108 +804,40 @@
       <c r="Q3" s="1"/>
     </row>
     <row r="4" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A4" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="B4" s="27" t="s">
-        <v>32</v>
-      </c>
-      <c r="C4" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="D4" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="E4" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="F4" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="G4" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="H4" s="27" t="s">
-        <v>38</v>
-      </c>
-      <c r="I4" s="27" t="s">
-        <v>39</v>
-      </c>
-      <c r="J4" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="K4" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="L4" s="27" t="s">
-        <v>42</v>
-      </c>
-      <c r="M4" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="N4" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="O4" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="P4" s="27" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q4" s="27" t="s">
-        <v>47</v>
-      </c>
-      <c r="R4" s="27" t="s">
-        <v>48</v>
-      </c>
-      <c r="S4" s="27" t="s">
-        <v>49</v>
-      </c>
-      <c r="T4" s="27" t="s">
-        <v>50</v>
-      </c>
-      <c r="U4" s="27" t="s">
-        <v>51</v>
-      </c>
-      <c r="V4" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="W4" s="27" t="s">
-        <v>53</v>
-      </c>
-      <c r="X4" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="Y4" s="27" t="s">
-        <v>55</v>
-      </c>
-      <c r="Z4" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="AA4" s="27" t="s">
-        <v>57</v>
-      </c>
-      <c r="AB4" s="27" t="s">
-        <v>58</v>
-      </c>
-      <c r="AC4" s="27" t="s">
-        <v>59</v>
-      </c>
-      <c r="AD4" s="27" t="s">
-        <v>60</v>
-      </c>
-      <c r="AE4" s="27" t="s">
-        <v>61</v>
-      </c>
-      <c r="AF4" s="27" t="s">
-        <v>62</v>
-      </c>
-      <c r="AG4" s="27" t="s">
-        <v>63</v>
-      </c>
-      <c r="AH4" s="27" t="s">
-        <v>64</v>
-      </c>
+      <c r="A4" s="26"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="26"/>
+      <c r="J4" s="26"/>
+      <c r="K4" s="26"/>
+      <c r="L4" s="26"/>
+      <c r="M4" s="26"/>
+      <c r="N4" s="26"/>
+      <c r="O4" s="26"/>
+      <c r="P4" s="26"/>
+      <c r="Q4" s="26"/>
+      <c r="R4" s="26"/>
+      <c r="S4" s="26"/>
+      <c r="T4" s="26"/>
+      <c r="U4" s="26"/>
+      <c r="V4" s="26"/>
+      <c r="W4" s="26"/>
+      <c r="X4" s="26"/>
+      <c r="Y4" s="26"/>
+      <c r="Z4" s="26"/>
+      <c r="AA4" s="26"/>
+      <c r="AB4" s="26"/>
+      <c r="AC4" s="26"/>
+      <c r="AD4" s="26"/>
+      <c r="AE4" s="26"/>
+      <c r="AF4" s="26"/>
+      <c r="AG4" s="26"/>
+      <c r="AH4" s="26"/>
       <c r="AK4" s="1"/>
       <c r="AL4" s="1"/>
       <c r="AM4" s="1"/>
@@ -1090,17 +914,13 @@
         <v>28</v>
       </c>
       <c r="X5" s="21" t="s">
-        <v>65</v>
+        <v>31</v>
       </c>
       <c r="Y5" s="21" t="s">
-        <v>66</v>
+        <v>32</v>
       </c>
-      <c r="Z5" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="AA5" s="21" t="s">
-        <v>68</v>
-      </c>
+      <c r="Z5" s="21"/>
+      <c r="AA5" s="21"/>
       <c r="AB5" s="21" t="s">
         <v>26</v>
       </c>

</xml_diff>

<commit_message>
Updated farmer import template
</commit_message>
<xml_diff>
--- a/src/assets/farmer-import/Template_list of farmers_NEW.xlsx
+++ b/src/assets/farmer-import/Template_list of farmers_NEW.xlsx
@@ -5,12 +5,12 @@
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bpaspalovski/IntellijProjects/inatrace/inatrace-fe/src/assets/farmer-import/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pecea/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F39A5A1B-2F8D-C844-B767-CB25519013C2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AE283D1-FF72-3F40-8178-18F7EB654631}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3440" yWindow="500" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -145,10 +145,10 @@
     </r>
   </si>
   <si>
-    <t>Area cultivated with coffee</t>
+    <t>Area cultivated with product of type</t>
   </si>
   <si>
-    <t>Number of coffee plants</t>
+    <t>Number of product type plants</t>
   </si>
 </sst>
 </file>
@@ -737,8 +737,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AN260"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="AA2" sqref="AA2"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>